<commit_message>
changes lvl1 + add bulb
</commit_message>
<xml_diff>
--- a/Esquema de Niveles/Levels.xlsx
+++ b/Esquema de Niveles/Levels.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\Documentos\GENIALITYXD USB\UDEA\SEMESTRE II\Informática II\Proyecto Final\Repositorio Proyecto\Esquema de Niveles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B630E5D2-DAC4-45C0-9B6B-A07940DD76F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E65EAD7-A190-41F0-9D81-FEE60AFA819A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7335" yWindow="885" windowWidth="20490" windowHeight="10920" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
+    <workbookView xWindow="15900" yWindow="3795" windowWidth="20730" windowHeight="11160" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
   </bookViews>
   <sheets>
     <sheet name="Level1" sheetId="1" r:id="rId1"/>
@@ -508,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827B320B-4A18-49AF-A0E1-B22C45EC2C53}">
-  <dimension ref="A1:AI35"/>
+  <dimension ref="A1:AL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AI9" sqref="AI9"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="79" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,7 +519,7 @@
     <col min="1" max="33" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -554,7 +554,7 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="3" t="s">
@@ -611,7 +611,7 @@
       <c r="AF2" s="3"/>
       <c r="AG2" s="1"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="3" t="s">
         <v>0</v>
@@ -658,7 +658,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="3">
         <v>0</v>
@@ -739,7 +739,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="3" t="s">
         <v>0</v>
@@ -784,7 +784,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>0</v>
@@ -879,7 +879,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="3" t="s">
         <v>0</v>
@@ -933,8 +933,11 @@
       <c r="AI7">
         <v>95</v>
       </c>
-    </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ7">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="3">
         <v>0</v>
@@ -988,8 +991,11 @@
       <c r="AI8">
         <v>94</v>
       </c>
-    </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ8">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="3" t="s">
         <v>0</v>
@@ -1049,8 +1055,17 @@
       <c r="AI9">
         <v>50</v>
       </c>
-    </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+      <c r="AJ9">
+        <v>51</v>
+      </c>
+      <c r="AK9">
+        <v>52</v>
+      </c>
+      <c r="AL9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="3">
         <v>0</v>
@@ -1107,7 +1122,7 @@
       </c>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="3" t="s">
         <v>0</v>
@@ -1160,7 +1175,7 @@
       </c>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1205,7 +1220,7 @@
       </c>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -1252,7 +1267,7 @@
       </c>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -1309,7 +1324,7 @@
       </c>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -1372,7 +1387,7 @@
       </c>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>

</xml_diff>

<commit_message>
config menu inicial + guardar partida + cargar partida + falta instruc init
</commit_message>
<xml_diff>
--- a/Esquema de Niveles/Levels.xlsx
+++ b/Esquema de Niveles/Levels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Documents\Documentos\GENIALITYXD USB\UDEA\SEMESTRE II\Informática II\Proyecto Final\Repositorio Proyecto\Esquema de Niveles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Desktop\RepoProyFinal\RepoProyFinal\Esquema de Niveles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E65EAD7-A190-41F0-9D81-FEE60AFA819A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C523F07-CCB9-4DEC-9EFD-AF6DE6F3D49F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15900" yWindow="3795" windowWidth="20730" windowHeight="11160" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="1" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
   </bookViews>
   <sheets>
     <sheet name="Level1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="33">
   <si>
     <t>-</t>
   </si>
@@ -82,6 +82,57 @@
   </si>
   <si>
     <t>Boton</t>
+  </si>
+  <si>
+    <t>Circ70</t>
+  </si>
+  <si>
+    <t>Eli71</t>
+  </si>
+  <si>
+    <t>Pen72</t>
+  </si>
+  <si>
+    <t>Cargador</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>B1</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>PY1</t>
+  </si>
+  <si>
+    <t>PY2</t>
+  </si>
+  <si>
+    <t>PYC1</t>
+  </si>
+  <si>
+    <t>|</t>
+  </si>
+  <si>
+    <t>V</t>
+  </si>
+  <si>
+    <t>^</t>
+  </si>
+  <si>
+    <t>CH1</t>
+  </si>
+  <si>
+    <t>83DOWN</t>
+  </si>
+  <si>
+    <t>82UP</t>
   </si>
 </sst>
 </file>
@@ -170,7 +221,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -189,6 +240,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -510,8 +567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{827B320B-4A18-49AF-A0E1-B22C45EC2C53}">
   <dimension ref="A1:AL35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="79" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+    <sheetView topLeftCell="V1" zoomScale="79" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="AH10" sqref="AH3:AL10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -783,6 +840,15 @@
       <c r="AI5">
         <v>97</v>
       </c>
+      <c r="AJ5" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL5" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
@@ -1121,6 +1187,12 @@
         <v>0</v>
       </c>
       <c r="AG10" s="1"/>
+      <c r="AH10" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI10">
+        <v>60</v>
+      </c>
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
@@ -2337,37 +2409,37 @@
       <c r="AF33" s="4"/>
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="C35" s="8" t="s">
+      <c r="C35" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-      <c r="F35" s="8"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-      <c r="J35" s="8"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="8"/>
-      <c r="M35" s="8"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="8"/>
-      <c r="P35" s="8"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="8"/>
-      <c r="S35" s="8"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="8"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="8"/>
-      <c r="X35" s="8"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="8"/>
-      <c r="AA35" s="8"/>
-      <c r="AB35" s="8"/>
-      <c r="AC35" s="8"/>
-      <c r="AD35" s="8"/>
-      <c r="AE35" s="8"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="10"/>
+      <c r="J35" s="10"/>
+      <c r="K35" s="10"/>
+      <c r="L35" s="10"/>
+      <c r="M35" s="10"/>
+      <c r="N35" s="10"/>
+      <c r="O35" s="10"/>
+      <c r="P35" s="10"/>
+      <c r="Q35" s="10"/>
+      <c r="R35" s="10"/>
+      <c r="S35" s="10"/>
+      <c r="T35" s="10"/>
+      <c r="U35" s="10"/>
+      <c r="V35" s="10"/>
+      <c r="W35" s="10"/>
+      <c r="X35" s="10"/>
+      <c r="Y35" s="10"/>
+      <c r="Z35" s="10"/>
+      <c r="AA35" s="10"/>
+      <c r="AB35" s="10"/>
+      <c r="AC35" s="10"/>
+      <c r="AD35" s="10"/>
+      <c r="AE35" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2379,18 +2451,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFBE286B-892F-4C46-B478-B5F3FDD42BA2}">
-  <dimension ref="A1:AG17"/>
+  <dimension ref="A1:AL17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AA11" sqref="AA11"/>
+    <sheetView tabSelected="1" zoomScale="69" workbookViewId="0">
+      <selection activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="33" width="3.85546875" customWidth="1"/>
+    <col min="1" max="15" width="3.85546875" customWidth="1"/>
+    <col min="16" max="16" width="4.85546875" customWidth="1"/>
+    <col min="17" max="17" width="3.85546875" customWidth="1"/>
+    <col min="18" max="18" width="5" customWidth="1"/>
+    <col min="19" max="33" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2425,852 +2501,1036 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
-      <c r="C2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="3">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J2" s="3">
-        <v>0</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M2" s="3">
-        <v>0</v>
-      </c>
-      <c r="N2" s="3"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="3"/>
-      <c r="Q2" s="3"/>
-      <c r="R2" s="3"/>
-      <c r="S2" s="3"/>
-      <c r="T2" s="3"/>
-      <c r="U2" s="3"/>
-      <c r="V2" s="3"/>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3"/>
-      <c r="Y2" s="3"/>
-      <c r="Z2" s="3"/>
-      <c r="AA2" s="3"/>
-      <c r="AB2" s="3"/>
-      <c r="AC2" s="3"/>
-      <c r="AD2" s="3"/>
-      <c r="AE2" s="3"/>
-      <c r="AF2" s="3"/>
+      <c r="C2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L2" s="8">
+        <v>0</v>
+      </c>
+      <c r="M2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N2" s="8">
+        <v>0</v>
+      </c>
+      <c r="O2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q2" s="8">
+        <v>0</v>
+      </c>
+      <c r="R2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="V2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W2" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="AG2" s="1"/>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH2" t="s">
+        <v>9</v>
+      </c>
+      <c r="AI2">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3"/>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I3" s="3"/>
-      <c r="J3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="L3" s="3"/>
-      <c r="M3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N3" s="3"/>
-      <c r="O3" s="3"/>
-      <c r="P3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="R3" s="3"/>
-      <c r="S3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="U3" s="3"/>
-      <c r="V3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="X3" s="3"/>
-      <c r="Y3" s="3"/>
-      <c r="Z3" s="3"/>
-      <c r="AA3" s="3"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="3"/>
-      <c r="AD3" s="3"/>
-      <c r="AE3" s="3"/>
-      <c r="AF3" s="3"/>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="8"/>
+      <c r="G3" s="8"/>
+      <c r="H3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="J3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L3" s="8"/>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="8"/>
+      <c r="R3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S3" s="8"/>
+      <c r="T3" s="8"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
+      <c r="X3" s="8"/>
+      <c r="Y3" s="8"/>
+      <c r="Z3" s="8"/>
+      <c r="AA3" s="8"/>
+      <c r="AB3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="8"/>
+      <c r="AD3" s="8"/>
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="AG3" s="1"/>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH3" t="s">
+        <v>10</v>
+      </c>
+      <c r="AI3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="3">
-        <v>0</v>
-      </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="R4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="V4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="3"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="3"/>
-      <c r="AC4" s="3"/>
-      <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
-      <c r="AF4" s="3"/>
+      <c r="B4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="L4" s="8">
+        <v>0</v>
+      </c>
+      <c r="M4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="O4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="R4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="S4" s="8">
+        <v>30</v>
+      </c>
+      <c r="T4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="U4" s="7"/>
+      <c r="V4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="W4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="X4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="9">
+        <v>30</v>
+      </c>
+      <c r="Z4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="AG4" s="1"/>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH4" t="s">
+        <v>11</v>
+      </c>
+      <c r="AI4">
+        <v>97</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>16</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>17</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
-      <c r="Z5" s="3"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="3"/>
-      <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
-      <c r="AF5" s="3"/>
+      <c r="B5" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="U5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="W5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="X5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z5" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA5" s="8"/>
+      <c r="AB5" s="8"/>
+      <c r="AC5" s="9"/>
+      <c r="AD5" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="8"/>
+      <c r="AF5" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="AG5" s="1"/>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH5" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="AI5">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="X6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="3"/>
+      <c r="B6" s="9">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+      <c r="N6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P6" s="8"/>
+      <c r="Q6" s="8"/>
+      <c r="R6" s="8"/>
+      <c r="S6" s="8"/>
+      <c r="T6" s="8"/>
+      <c r="U6" s="8"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Y6" s="8"/>
+      <c r="Z6" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="9"/>
+      <c r="AD6" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="8"/>
+      <c r="AF6" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="AG6" s="1"/>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH6" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI6">
+        <v>95</v>
+      </c>
+      <c r="AJ6">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="3"/>
-      <c r="D7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="U7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
-      <c r="Z7" s="3"/>
-      <c r="AA7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="3"/>
-      <c r="AC7" s="3"/>
-      <c r="AD7" s="3"/>
-      <c r="AE7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="3"/>
+      <c r="B7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+      <c r="L7" s="8"/>
+      <c r="M7" s="8"/>
+      <c r="N7" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="O7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q7" s="8"/>
+      <c r="R7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="S7" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="T7" s="8"/>
+      <c r="U7" s="8"/>
+      <c r="V7" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="W7" s="8"/>
+      <c r="X7" s="8"/>
+      <c r="Y7" s="8"/>
+      <c r="Z7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA7" s="8"/>
+      <c r="AB7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE7" s="8"/>
+      <c r="AF7" s="8" t="s">
+        <v>0</v>
+      </c>
       <c r="AG7" s="1"/>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.25">
+      <c r="AH7" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI7">
+        <v>94</v>
+      </c>
+      <c r="AJ7">
+        <v>93</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>31</v>
+      </c>
+      <c r="AL7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3" t="s">
+      <c r="B8" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="8">
+        <v>0</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8"/>
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+      <c r="L8" s="8"/>
+      <c r="M8" s="8"/>
+      <c r="N8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q8" s="8"/>
+      <c r="R8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S8" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="T8" s="8"/>
+      <c r="U8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3" t="s">
+      <c r="V8" s="8"/>
+      <c r="W8" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3" t="s">
+      <c r="X8" s="8"/>
+      <c r="Y8" s="8"/>
+      <c r="Z8" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA8" s="8"/>
+      <c r="AB8" s="8"/>
+      <c r="AC8" s="9"/>
+      <c r="AD8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE8" s="8"/>
+      <c r="AF8" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG8" s="1"/>
+      <c r="AH8" t="s">
+        <v>15</v>
+      </c>
+      <c r="AI8">
+        <v>50</v>
+      </c>
+      <c r="AJ8">
+        <v>51</v>
+      </c>
+      <c r="AK8">
+        <v>52</v>
+      </c>
+      <c r="AL8">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="9">
+        <v>0</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L9" s="8"/>
+      <c r="M9" s="8"/>
+      <c r="N9" s="8"/>
+      <c r="O9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S9" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T9" s="8"/>
+      <c r="U9" s="8"/>
+      <c r="V9" s="8"/>
+      <c r="W9" s="8"/>
+      <c r="X9" s="8"/>
+      <c r="Y9" s="8"/>
+      <c r="Z9" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA9" s="8"/>
+      <c r="AB9" s="8"/>
+      <c r="AC9" s="9"/>
+      <c r="AD9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF9" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG9" s="1"/>
+      <c r="AH9" t="s">
+        <v>19</v>
+      </c>
+      <c r="AI9">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+      <c r="L10" s="8"/>
+      <c r="M10" s="8"/>
+      <c r="N10" s="8"/>
+      <c r="O10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="S10" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="T10" s="8"/>
+      <c r="U10" s="8"/>
+      <c r="V10" s="8"/>
+      <c r="W10" s="8"/>
+      <c r="X10" s="8"/>
+      <c r="Y10" s="8"/>
+      <c r="Z10" s="8"/>
+      <c r="AA10" s="8"/>
+      <c r="AB10" s="8"/>
+      <c r="AC10" s="9"/>
+      <c r="AD10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG10" s="1"/>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3" t="s">
+      <c r="K11" s="8"/>
+      <c r="L11" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="S8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
-      <c r="Z8" s="3"/>
-      <c r="AA8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="3"/>
-      <c r="AC8" s="3"/>
-      <c r="AD8" s="3"/>
-      <c r="AE8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="3"/>
-      <c r="AG8" s="1"/>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
-      <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="3"/>
-      <c r="D9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3" t="s">
+      <c r="M11" s="8"/>
+      <c r="N11" s="8"/>
+      <c r="O11" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="P11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R11" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S11" s="8"/>
+      <c r="T11" s="8"/>
+      <c r="U11" s="8"/>
+      <c r="V11" s="8"/>
+      <c r="W11" s="8"/>
+      <c r="X11" s="8"/>
+      <c r="Y11" s="8"/>
+      <c r="Z11" s="8"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="8"/>
+      <c r="AC11" s="9"/>
+      <c r="AD11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE11" s="8"/>
+      <c r="AF11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AG11" s="1"/>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="R9" s="3"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="3"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
-      <c r="Z9" s="3"/>
-      <c r="AA9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="3"/>
-      <c r="AC9" s="3"/>
-      <c r="AD9" s="3"/>
-      <c r="AE9" s="3">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="1"/>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="3"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="3">
-        <v>0</v>
-      </c>
-      <c r="AB10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
-      <c r="AF10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG10" s="1"/>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="3">
-        <v>0</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E11" s="3" t="s">
+      <c r="L12" s="8"/>
+      <c r="M12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="P12" s="8"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="8"/>
+      <c r="S12" s="8"/>
+      <c r="T12" s="8"/>
+      <c r="U12" s="8"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="X12" s="8"/>
+      <c r="Y12" s="8"/>
+      <c r="Z12" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
-      <c r="R11" s="3"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="3"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="3"/>
-      <c r="Z11" s="3"/>
-      <c r="AA11" s="6"/>
-      <c r="AB11" s="3"/>
-      <c r="AC11" s="3">
-        <v>0</v>
-      </c>
-      <c r="AD11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AE11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG11" s="1"/>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="3"/>
-      <c r="AB12" s="3"/>
-      <c r="AC12" s="3"/>
-      <c r="AD12" s="3"/>
-      <c r="AE12" s="3"/>
-      <c r="AF12" s="3" t="s">
+      <c r="AA12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE12" s="8"/>
+      <c r="AF12" s="8" t="s">
         <v>0</v>
       </c>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
-      <c r="Z13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="3"/>
-      <c r="AB13" s="3"/>
-      <c r="AC13" s="3"/>
-      <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
-      <c r="AF13" s="3" t="s">
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8"/>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8"/>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T13" s="8"/>
+      <c r="U13" s="8"/>
+      <c r="V13" s="8"/>
+      <c r="W13" s="8"/>
+      <c r="X13" s="8"/>
+      <c r="Y13" s="8"/>
+      <c r="Z13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA13" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB13" s="8"/>
+      <c r="AC13" s="9"/>
+      <c r="AD13" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE13" s="8"/>
+      <c r="AF13" s="8" t="s">
         <v>0</v>
       </c>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3"/>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3"/>
-      <c r="O14" s="3"/>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3"/>
-      <c r="R14" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="S14" s="3"/>
-      <c r="T14" s="3"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y14" s="3"/>
-      <c r="Z14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="3"/>
-      <c r="AB14" s="3"/>
-      <c r="AC14" s="3"/>
-      <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
-      <c r="AF14" s="3">
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
+      <c r="L14" s="8"/>
+      <c r="M14" s="8"/>
+      <c r="N14" s="8"/>
+      <c r="O14" s="8"/>
+      <c r="P14" s="8"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S14" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="T14" s="8"/>
+      <c r="U14" s="8"/>
+      <c r="V14" s="8"/>
+      <c r="W14" s="8"/>
+      <c r="X14" s="8"/>
+      <c r="Y14" s="8"/>
+      <c r="Z14" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA14" s="8"/>
+      <c r="AB14" s="8"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE14" s="8"/>
+      <c r="AF14" s="8" t="s">
         <v>0</v>
       </c>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="M15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="N15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="O15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="P15" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q15" s="3"/>
-      <c r="R15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S15" s="3"/>
-      <c r="T15" s="3"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="Y15" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="3"/>
-      <c r="AB15" s="3"/>
-      <c r="AC15" s="3"/>
-      <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
-      <c r="AF15" s="3" t="s">
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
+      <c r="L15" s="8"/>
+      <c r="M15" s="8"/>
+      <c r="N15" s="8"/>
+      <c r="O15" s="8"/>
+      <c r="P15" s="8"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T15" s="8"/>
+      <c r="U15" s="8"/>
+      <c r="V15" s="8"/>
+      <c r="W15" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="X15" s="8"/>
+      <c r="Y15" s="8"/>
+      <c r="Z15" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB15" s="8"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE15" s="8"/>
+      <c r="AF15" s="8" t="s">
         <v>0</v>
       </c>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="G16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="I16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="J16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="K16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="L16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="M16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="N16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="R16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="S16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="T16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="U16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="V16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="W16" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
-      <c r="Z16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AB16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AC16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AD16" s="3">
-        <v>0</v>
-      </c>
-      <c r="AE16" s="3" t="s">
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="8"/>
+      <c r="E16" s="8"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="8"/>
+      <c r="H16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="J16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="K16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="M16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="N16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="O16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="P16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="R16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="S16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="T16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="U16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="V16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="W16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="X16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="Z16" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="AA16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AB16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="AE16" s="8" t="s">
         <v>0</v>
       </c>
       <c r="AF16" s="4"/>

</xml_diff>

<commit_message>
new branch for lvl 3 + instruc imgs
</commit_message>
<xml_diff>
--- a/Esquema de Niveles/Levels.xlsx
+++ b/Esquema de Niveles/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Desktop\RepoProyFinal\RepoProyFinal\Esquema de Niveles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713330AF-D1DE-4188-9750-1999E5992F4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA15F105-98FE-4CBD-9CFE-F11331DAB2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="2" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
   </bookViews>
@@ -3617,7 +3617,7 @@
   <dimension ref="A1:AL17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13"/>
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
creacion mapa 3 + falta vidas grafica UI + analize plats 80 81 & lvl3 new stuff
</commit_message>
<xml_diff>
--- a/Esquema de Niveles/Levels.xlsx
+++ b/Esquema de Niveles/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Desktop\RepoProyFinal\RepoProyFinal\Esquema de Niveles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA15F105-98FE-4CBD-9CFE-F11331DAB2B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DF97A7-231F-4612-8D54-64240FE0DA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="2" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="677" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="48">
   <si>
     <t>-</t>
   </si>
@@ -172,6 +172,12 @@
   </si>
   <si>
     <t>PX</t>
+  </si>
+  <si>
+    <t>81RIGHT</t>
+  </si>
+  <si>
+    <t>80LEFT</t>
   </si>
 </sst>
 </file>
@@ -3614,10 +3620,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C851EC-8CFE-4116-8AA8-E06224E2E1E3}">
-  <dimension ref="A1:AL17"/>
+  <dimension ref="A1:AN17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="AJ9" sqref="AJ9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3629,7 +3635,7 @@
     <col min="19" max="33" width="3.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -3664,7 +3670,7 @@
       <c r="AF1" s="1"/>
       <c r="AG1" s="1"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="2"/>
       <c r="C2" s="9" t="s">
@@ -3763,7 +3769,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="9" t="s">
         <v>0</v>
@@ -3820,7 +3826,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="9" t="s">
         <v>0</v>
@@ -3919,7 +3925,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="9" t="s">
         <v>0</v>
@@ -4010,7 +4016,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="9" t="s">
         <v>0</v>
@@ -4030,12 +4036,15 @@
         <v>2</v>
       </c>
       <c r="I6" s="9"/>
-      <c r="J6" s="9"/>
       <c r="K6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="L6" s="9"/>
-      <c r="M6" s="9"/>
+      <c r="M6" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="N6" s="9"/>
       <c r="O6" s="9"/>
       <c r="P6" s="9" t="s">
@@ -4047,12 +4056,15 @@
       </c>
       <c r="S6" s="9"/>
       <c r="T6" s="9"/>
-      <c r="U6" s="9"/>
-      <c r="V6" s="9"/>
+      <c r="U6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="V6" s="9" t="s">
+        <v>22</v>
+      </c>
       <c r="W6" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="X6" s="9"/>
+        <v>2</v>
+      </c>
       <c r="Y6" s="9"/>
       <c r="Z6" s="9" t="s">
         <v>2</v>
@@ -4082,7 +4094,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="9">
         <v>0</v>
@@ -4102,14 +4114,13 @@
         <v>2</v>
       </c>
       <c r="I7" s="9"/>
-      <c r="J7" s="9" t="s">
+      <c r="K7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="K7" s="9"/>
-      <c r="L7" s="9" t="s">
+      <c r="L7" s="9"/>
+      <c r="M7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="M7" s="9"/>
       <c r="N7" s="9"/>
       <c r="O7" s="9"/>
       <c r="P7" s="9" t="s">
@@ -4121,12 +4132,11 @@
       </c>
       <c r="S7" s="9"/>
       <c r="T7" s="9"/>
-      <c r="U7" s="9"/>
-      <c r="V7" s="9" t="s">
+      <c r="U7" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="W7" s="9"/>
-      <c r="X7" s="9" t="s">
+      <c r="V7" s="9"/>
+      <c r="W7" s="9" t="s">
         <v>35</v>
       </c>
       <c r="Y7" s="9"/>
@@ -4161,8 +4171,14 @@
       <c r="AL7" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AM7" t="s">
+        <v>46</v>
+      </c>
+      <c r="AN7" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="9" t="s">
         <v>0</v>
@@ -4178,7 +4194,9 @@
       <c r="G8" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
@@ -4230,7 +4248,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="9" t="s">
         <v>0</v>
@@ -4272,9 +4290,7 @@
       <c r="W9" s="9"/>
       <c r="X9" s="9"/>
       <c r="Y9" s="9"/>
-      <c r="Z9" s="9" t="s">
-        <v>2</v>
-      </c>
+      <c r="Z9" s="9"/>
       <c r="AA9" s="9"/>
       <c r="AB9" s="9" t="s">
         <v>0</v>
@@ -4298,8 +4314,11 @@
       <c r="AI9">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
+      <c r="AJ9">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="9">
         <v>0</v>
@@ -4380,7 +4399,7 @@
       </c>
       <c r="AG10" s="1"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="9" t="s">
         <v>0</v>
@@ -4441,15 +4460,13 @@
       </c>
       <c r="AG11" s="1"/>
     </row>
-    <row r="12" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="9" t="s">
         <v>0</v>
       </c>
       <c r="C12" s="9"/>
-      <c r="D12" s="9" t="s">
-        <v>0</v>
-      </c>
+      <c r="D12" s="9"/>
       <c r="E12" s="9"/>
       <c r="F12" s="9"/>
       <c r="G12" s="9">
@@ -4498,7 +4515,7 @@
       </c>
       <c r="AG12" s="1"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="9">
         <v>0</v>
@@ -4547,7 +4564,7 @@
       </c>
       <c r="AG13" s="1"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="9" t="s">
         <v>0</v>
@@ -4608,7 +4625,7 @@
       </c>
       <c r="AG14" s="1"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="9" t="s">
         <v>0</v>
@@ -4663,7 +4680,7 @@
       </c>
       <c r="AG15" s="1"/>
     </row>
-    <row r="16" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="9" t="s">
         <v>30</v>

</xml_diff>

<commit_message>
casi fin lvl3 (sistema vidas + lvls + fin game done) falta mov pendular (por ahora es MCUA) + editar img fin de juego
</commit_message>
<xml_diff>
--- a/Esquema de Niveles/Levels.xlsx
+++ b/Esquema de Niveles/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Desktop\RepoProyFinal\RepoProyFinal\Esquema de Niveles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87DF97A7-231F-4612-8D54-64240FE0DA26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BE5A18-2868-4C1C-98C0-99331C9C0739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="2" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
   </bookViews>
@@ -286,10 +286,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2450,37 +2450,37 @@
       <c r="AF33" s="4"/>
     </row>
     <row r="35" spans="2:32" x14ac:dyDescent="0.25">
-      <c r="C35" s="10" t="s">
+      <c r="C35" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="10"/>
-      <c r="E35" s="10"/>
-      <c r="F35" s="10"/>
-      <c r="G35" s="10"/>
-      <c r="H35" s="10"/>
-      <c r="I35" s="10"/>
-      <c r="J35" s="10"/>
-      <c r="K35" s="10"/>
-      <c r="L35" s="10"/>
-      <c r="M35" s="10"/>
-      <c r="N35" s="10"/>
-      <c r="O35" s="10"/>
-      <c r="P35" s="10"/>
-      <c r="Q35" s="10"/>
-      <c r="R35" s="10"/>
-      <c r="S35" s="10"/>
-      <c r="T35" s="10"/>
-      <c r="U35" s="10"/>
-      <c r="V35" s="10"/>
-      <c r="W35" s="10"/>
-      <c r="X35" s="10"/>
-      <c r="Y35" s="10"/>
-      <c r="Z35" s="10"/>
-      <c r="AA35" s="10"/>
-      <c r="AB35" s="10"/>
-      <c r="AC35" s="10"/>
-      <c r="AD35" s="10"/>
-      <c r="AE35" s="10"/>
+      <c r="D35" s="11"/>
+      <c r="E35" s="11"/>
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11"/>
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="11"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
+      <c r="U35" s="11"/>
+      <c r="V35" s="11"/>
+      <c r="W35" s="11"/>
+      <c r="X35" s="11"/>
+      <c r="Y35" s="11"/>
+      <c r="Z35" s="11"/>
+      <c r="AA35" s="11"/>
+      <c r="AB35" s="11"/>
+      <c r="AC35" s="11"/>
+      <c r="AD35" s="11"/>
+      <c r="AE35" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3623,7 +3623,7 @@
   <dimension ref="A1:AN17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="AJ9" sqref="AJ9"/>
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3814,8 +3814,8 @@
       </c>
       <c r="AC3" s="9"/>
       <c r="AD3" s="9"/>
-      <c r="AE3" s="9" t="s">
-        <v>0</v>
+      <c r="AE3" s="9">
+        <v>40</v>
       </c>
       <c r="AF3" s="9"/>
       <c r="AG3" s="1"/>
@@ -4005,8 +4005,8 @@
         <v>0</v>
       </c>
       <c r="AE5" s="9"/>
-      <c r="AF5" s="9" t="s">
-        <v>0</v>
+      <c r="AF5" s="9">
+        <v>40</v>
       </c>
       <c r="AG5" s="1"/>
       <c r="AH5" s="9" t="s">
@@ -4014,6 +4014,12 @@
       </c>
       <c r="AI5">
         <v>96</v>
+      </c>
+      <c r="AJ5">
+        <v>86</v>
+      </c>
+      <c r="AK5">
+        <v>76</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -4499,7 +4505,7 @@
         <v>0</v>
       </c>
       <c r="AB12" s="9">
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="AC12" s="9" t="s">
         <v>0</v>
@@ -4537,11 +4543,15 @@
       <c r="M13" s="9"/>
       <c r="N13" s="9"/>
       <c r="O13" s="9"/>
-      <c r="P13" s="9"/>
+      <c r="P13" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="Q13" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="R13" s="9"/>
+      <c r="R13" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="S13" s="9"/>
       <c r="T13" s="9"/>
       <c r="U13" s="9"/>
@@ -4595,7 +4605,9 @@
       <c r="P14" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="Q14" s="9"/>
+      <c r="Q14" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="R14" s="9" t="s">
         <v>39</v>
       </c>
@@ -4694,8 +4706,8 @@
       <c r="E16" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="F16" s="9" t="s">
-        <v>0</v>
+      <c r="F16" s="9">
+        <v>50</v>
       </c>
       <c r="G16" s="9" t="s">
         <v>0</v>
@@ -4768,7 +4780,7 @@
       <c r="AE16" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AF16" s="11"/>
+      <c r="AF16" s="10"/>
       <c r="AG16" s="1"/>
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added instruc for canon + added logica varios users + fin pruebas de lvls + fin pruebas juego = Fin Juego
</commit_message>
<xml_diff>
--- a/Esquema de Niveles/Levels.xlsx
+++ b/Esquema de Niveles/Levels.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Juan Diego\Desktop\RepoProyFinal\RepoProyFinal\Esquema de Niveles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2BE5A18-2868-4C1C-98C0-99331C9C0739}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BA97721-EF00-4C39-B2E6-C7146B6159F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="10920" activeTab="2" xr2:uid="{9A250328-CCC3-498E-AE7A-545EE819592A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="682" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="49">
   <si>
     <t>-</t>
   </si>
@@ -178,6 +178,9 @@
   </si>
   <si>
     <t>80LEFT</t>
+  </si>
+  <si>
+    <t>PY3</t>
   </si>
 </sst>
 </file>
@@ -2495,7 +2498,7 @@
   <dimension ref="A1:AL17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P13" sqref="P13"/>
+      <selection activeCell="AC14" sqref="AC14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3142,7 +3145,7 @@
         <v>26</v>
       </c>
       <c r="S9" s="7" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="T9" s="7"/>
       <c r="U9" s="7"/>
@@ -3209,13 +3212,13 @@
         <v>26</v>
       </c>
       <c r="Q10" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="R10" s="7" t="s">
         <v>26</v>
       </c>
       <c r="S10" s="7" t="s">
-        <v>25</v>
+        <v>48</v>
       </c>
       <c r="T10" s="7"/>
       <c r="U10" s="7"/>
@@ -3423,7 +3426,7 @@
         <v>2</v>
       </c>
       <c r="S14" s="7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="T14" s="7"/>
       <c r="U14" s="7"/>
@@ -3486,7 +3489,7 @@
       </c>
       <c r="AB15" s="7"/>
       <c r="AC15" s="8"/>
-      <c r="AD15" s="7" t="s">
+      <c r="AD15" s="7">
         <v>0</v>
       </c>
       <c r="AE15" s="7"/>
@@ -3622,8 +3625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25C851EC-8CFE-4116-8AA8-E06224E2E1E3}">
   <dimension ref="A1:AN17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3758,9 +3761,7 @@
       <c r="AE2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="AF2" s="9" t="s">
-        <v>37</v>
-      </c>
+      <c r="AF2" s="9"/>
       <c r="AG2" s="1"/>
       <c r="AH2" t="s">
         <v>9</v>
@@ -3898,8 +3899,8 @@
         <v>0</v>
       </c>
       <c r="AA4" s="9"/>
-      <c r="AB4" s="9" t="s">
-        <v>0</v>
+      <c r="AB4" s="9">
+        <v>40</v>
       </c>
       <c r="AC4" s="9"/>
       <c r="AD4" s="9" t="s">
@@ -4077,7 +4078,7 @@
       </c>
       <c r="AA6" s="9"/>
       <c r="AB6" s="9" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="AC6" s="9"/>
       <c r="AD6" s="9" t="s">
@@ -4505,7 +4506,7 @@
         <v>0</v>
       </c>
       <c r="AB12" s="9">
-        <v>40</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="9" t="s">
         <v>0</v>

</xml_diff>